<commit_message>
AutomationTest-FinalProject: Add Test Listener
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\automation-test-group1\src\data\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>TCs</t>
   </si>
@@ -146,7 +146,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +250,91 @@
       <sz val="13"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +382,68 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -455,11 +599,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,6 +811,63 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="26" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="30" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,13 +1189,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="22.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="26.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="42.21875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="22.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -914,10 +1241,10 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="30" t="s">
         <v>33</v>
       </c>
     </row>
@@ -964,10 +1291,10 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -990,10 +1317,10 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="36" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1012,10 +1339,10 @@
       <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="39" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1036,10 +1363,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="42" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1060,10 +1387,10 @@
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="45" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1077,7 +1404,7 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="46" t="s">
         <v>34</v>
       </c>
       <c r="I9"/>

</xml_diff>

<commit_message>
AutomationTest-FinalProject: Write Test Cases For Edit Customer Fuction
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\automation-test-group1\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanlangunivn-my.sharepoint.com/personal/nhung_207ct28289_vanlanguni_vn/Documents/Automation Test/eclipse/automation-test-group1/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_39F6CD85D4EBBCD709F5F6220A7D857DCA3559DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDA1E68B-02D0-43B0-A0DC-035C2F900163}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeleteCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="EditCustomer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
   <si>
     <t>TCs</t>
   </si>
@@ -140,14 +131,131 @@
   </si>
   <si>
     <t>7/7</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_01</t>
+  </si>
+  <si>
+    <t>Test that Administrator can edit customer successfully and system displays "Sucessfully Updated" with all valid required fields edited</t>
+  </si>
+  <si>
+    <t>Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Successfully Updated</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_02</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 1 character and Description has 10 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_03</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 50 characters and Description has 10 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_04</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 5 characters and Description has 0 character in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_05</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 5 characters and Description has 255 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_06</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_07</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_08</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_09</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_10</t>
+  </si>
+  <si>
+    <t>Verify that the system reloads the page and displays the Customers page when the Administrator edits invalid data into input fields then closes 'Edit Customer' form by clicking 'Cancel' button</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/time/viewCustomers</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_11</t>
+  </si>
+  <si>
+    <t>Verify that the system reloads the page and displays the Customers page when the Administrator edits valid data into input fields then closes 'Edit Customer' form by clicking 'Cancel' button</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Welcome To</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Company</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Saigon Tourist Saigon Tourist Saigo</t>
+  </si>
+  <si>
+    <t>Saigo</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tou</t>
+  </si>
+  <si>
+    <t>ACME Ltd</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Saigon Tourist Saigon Tourist Saigon</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Required' text under customer name textbox when Administrator tries to save form with blank input to 'Name' textbox after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Already exists' text under customer name textbox when Administrator tries to save form with duplicated Name in the system after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Should not exceed 50 characters' text under customer description textbox when Administrator tries to enter on Name more than 50 characters in length after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Should not exceed 255 characters' text under customer description textarea when Administrator tries to enter on Description more than 255 characters in length after editing</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Already exists</t>
+  </si>
+  <si>
+    <t>Should not exceed 50 characters</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Should not exceed 255 characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="73" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +359,96 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <name val="Times New Roman"/>
       <sz val="12.0"/>
     </font>
@@ -330,11 +528,71 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +641,56 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill>
         <fgColor indexed="17"/>
       </patternFill>
@@ -442,8 +750,58 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="39">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -600,6 +958,228 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
       <top style="thin"/>
     </border>
     <border>
@@ -729,7 +1309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -755,7 +1335,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -773,6 +1353,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -812,61 +1404,166 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="26" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="30" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="24" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="28" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="28" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="32" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="32" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="25" borderId="32" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="36" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="36" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="27" borderId="36" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="40" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="40" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="29" borderId="40" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="44" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="31" borderId="44" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="48" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="48" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="33" borderId="48" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="52" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="52" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="35" borderId="52" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="56" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="56" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="37" borderId="56" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="60" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="60" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="39" borderId="60" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="64" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="64" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="41" borderId="64" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1182,23 +1879,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection sqref="A1:H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="20.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="42.21875" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="1" width="22.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="42.1796875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="22.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.90625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="26.6328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.6328125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1241,14 +1940,14 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -1265,14 +1964,14 @@
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -1291,14 +1990,14 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -1317,14 +2016,14 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1339,14 +2038,14 @@
       <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
@@ -1363,14 +2062,14 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
@@ -1387,14 +2086,14 @@
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1404,7 +2103,7 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="31" t="s">
         <v>34</v>
       </c>
       <c r="I9"/>
@@ -1413,4 +2112,311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E731B3F8-B060-4481-934E-7DC39C925434}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="25.453125" collapsed="true"/>
+    <col min="2" max="8" customWidth="true" width="35.81640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="131" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="79" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="114.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="82" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AutomationTest-FinalProject: Write Test Cases For Employee Reports Function
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -8,25 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanlangunivn-my.sharepoint.com/personal/nhung_207ct28289_vanlanguni_vn/Documents/Automation Test/eclipse/automation-test-group1/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_39F6CD85D4EBBCD709F5F6220A7D857DCA3559DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDA1E68B-02D0-43B0-A0DC-035C2F900163}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="11_39F6CD85D4EBBCD709F5F6220A7D857DCA3559DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0871463-F3B0-4537-AD68-F3BFE77EB402}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeleteCustomer" sheetId="1" r:id="rId1"/>
     <sheet name="EditCustomer" sheetId="2" r:id="rId2"/>
+    <sheet name="EmployeeReports" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="108">
   <si>
     <t>TCs</t>
   </si>
@@ -248,6 +260,108 @@
   </si>
   <si>
     <t>Should not exceed 255 characters</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_01</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_02</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_03</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_04</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_05</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_06</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_07</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_08</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_09</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee and the project name.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and a specific activity in the project.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and the project date range in the project.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, a specific activity, and project date range in the project.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, and turn on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, project's activity, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, the project's activity, project date range, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>ACME</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Approved Timesheets</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>2023-08-13</t>
+  </si>
+  <si>
+    <t>2023-08-20</t>
+  </si>
+  <si>
+    <t>0/10</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>orangehrm-paper-container</t>
+  </si>
+  <si>
+    <t>class jdk.proxy2.$Proxy19</t>
+  </si>
+  <si>
+    <t>8/10</t>
+  </si>
+  <si>
+    <t>9/10</t>
   </si>
 </sst>
 </file>
@@ -255,7 +369,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="73" x14ac:knownFonts="1">
+  <fonts count="106" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +563,26 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <name val="Times New Roman"/>
       <sz val="12.0"/>
     </font>
@@ -591,8 +725,135 @@
       <sz val="13.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="42">
+  <fills count="61">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,6 +952,11 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill>
         <fgColor indexed="17"/>
       </patternFill>
@@ -800,8 +1066,98 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="65">
+  <borders count="111">
     <border>
       <left/>
       <right/>
@@ -1108,6 +1464,234 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
       <top style="thin"/>
     </border>
     <border>
@@ -1309,7 +1893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1362,9 +1946,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1467,103 +2048,235 @@
     <xf numFmtId="0" fontId="39" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="24" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="28" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="28" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="32" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="32" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="25" borderId="32" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="36" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="36" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="27" borderId="36" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="40" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="40" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="29" borderId="40" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="44" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="31" borderId="44" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="48" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="48" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="33" borderId="48" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="52" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="52" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="35" borderId="52" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="56" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="56" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="37" borderId="56" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="60" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="60" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="39" borderId="60" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="64" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="64" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="41" borderId="64" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="26" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="26" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="38" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="42" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="42" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="30" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="46" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="46" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="32" borderId="46" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="50" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="50" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="34" borderId="50" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="54" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="54" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="36" borderId="54" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="58" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="58" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="38" borderId="58" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="62" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="62" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="40" borderId="62" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="42" borderId="66" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="70" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="74" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="74" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="44" borderId="74" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="78" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="78" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="46" borderId="78" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="82" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="82" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="48" borderId="82" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="86" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="86" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="50" borderId="86" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="90" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="90" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="52" borderId="90" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="94" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="94" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="54" borderId="94" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="98" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="98" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="56" borderId="98" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="102" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="102" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="58" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="106" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="106" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="60" borderId="106" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="110" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1581,6 +2294,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1940,10 +2657,10 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1990,10 +2707,10 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2016,10 +2733,10 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2038,10 +2755,10 @@
       <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2062,10 +2779,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2086,10 +2803,10 @@
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2103,7 +2820,7 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="30" t="s">
         <v>34</v>
       </c>
       <c r="I9"/>
@@ -2118,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E731B3F8-B060-4481-934E-7DC39C925434}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="A1:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2173,10 +2890,10 @@
       <c r="F2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2197,10 +2914,10 @@
       <c r="F3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="35" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2221,10 +2938,10 @@
       <c r="F4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="37" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2243,10 +2960,10 @@
       <c r="F5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="39" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2267,10 +2984,10 @@
       <c r="F6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="41" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2289,10 +3006,10 @@
       <c r="F7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="43" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2313,10 +3030,10 @@
       <c r="F8" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="45" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2337,10 +3054,10 @@
       <c r="F9" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="74" t="s">
+      <c r="G9" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="47" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2361,10 +3078,10 @@
       <c r="F10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="77" t="s">
+      <c r="G10" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="79" t="s">
+      <c r="H10" s="49" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2382,13 +3099,13 @@
       <c r="E11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="80" t="s">
+      <c r="G11" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="82" t="s">
+      <c r="H11" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2406,17 +3123,357 @@
       <c r="E12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="83" t="s">
+      <c r="G12" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="85" t="s">
+      <c r="H12" s="53" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9486D730-61B3-4FC6-88FC-6911F5E0A3BE}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.54296875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="22.26953125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.1796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.08984375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="33.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.26953125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="101" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="103" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="104" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="106" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" s="110" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="59"/>
+      <c r="I6" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="113" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="115" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="60" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="118" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="60" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="121" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="60" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="122" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="124" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="60" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="127" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="128" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <phoneticPr fontId="42" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AutomationTest-FinalProject: Add Test Listener, Reporter Log And Update Old Methods
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanlangunivn-my.sharepoint.com/personal/nhung_207ct28289_vanlanguni_vn/Documents/Automation Test/eclipse/automation-test-group1/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="11_39F6CD85D4EBBCD709F5F6220A7D857DCA3559DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0871463-F3B0-4537-AD68-F3BFE77EB402}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="11_39F6CD85D4EBBCD709F5F6220A7D857DCA3559DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4725116F-7FE2-40BA-A26C-F8B5E8D19EB8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="105">
   <si>
     <t>TCs</t>
   </si>
@@ -346,19 +346,10 @@
     <t>2023-08-20</t>
   </si>
   <si>
-    <t>0/10</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>orangehrm-paper-container</t>
-  </si>
-  <si>
-    <t>class jdk.proxy2.$Proxy19</t>
-  </si>
-  <si>
-    <t>8/10</t>
   </si>
   <si>
     <t>9/10</t>
@@ -369,7 +360,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="106" x14ac:knownFonts="1">
+  <fonts count="183" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,17 +569,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -610,14 +674,6 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
@@ -636,14 +692,6 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
@@ -727,6 +775,14 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
@@ -758,14 +814,6 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
@@ -849,11 +897,294 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="61">
+  <fills count="106">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,6 +1288,51 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill>
         <fgColor indexed="17"/>
       </patternFill>
@@ -1156,8 +1532,188 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="111">
+  <borders count="212">
     <border>
       <left/>
       <right/>
@@ -1494,6 +2050,555 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
       <top style="thin"/>
     </border>
     <border>
@@ -1893,7 +2998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2060,30 +3165,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2093,190 +3177,421 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="26" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="34" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="26" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="38" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="38" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="42" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="42" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="30" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="46" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="46" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="32" borderId="46" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="50" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="50" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="34" borderId="50" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="54" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="54" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="36" borderId="54" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="58" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="58" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="38" borderId="58" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="62" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="62" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="40" borderId="62" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="42" borderId="66" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="70" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="74" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="74" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="44" borderId="74" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="78" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="78" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="46" borderId="78" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="82" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="82" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="48" borderId="82" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="86" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="86" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="50" borderId="86" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="90" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="90" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="52" borderId="90" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="94" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="94" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="54" borderId="94" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="98" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="98" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="56" borderId="98" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="102" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="102" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="101" fillId="58" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="106" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="106" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="104" fillId="60" borderId="106" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="110" xfId="0" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="44" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="25" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="27" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="29" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="35" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="39" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="39" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="31" borderId="39" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="43" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="47" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="47" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="33" borderId="47" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="51" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="55" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="55" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="35" borderId="55" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="59" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="59" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="37" borderId="59" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="63" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="63" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="39" borderId="63" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="67" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="67" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="41" borderId="67" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="71" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="71" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="43" borderId="71" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="75" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="75" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="45" borderId="75" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="79" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="79" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="47" borderId="79" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="83" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="83" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="49" borderId="83" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="87" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="87" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="51" borderId="87" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="91" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="95" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="95" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="53" borderId="95" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="99" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="99" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="55" borderId="99" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="103" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="103" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="57" borderId="103" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="107" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="107" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="59" borderId="107" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="111" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="111" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="61" borderId="111" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="63" borderId="115" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="119" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="119" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="65" borderId="119" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="67" borderId="123" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="127" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="127" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="69" borderId="127" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="131" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="135" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="135" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="71" borderId="135" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="139" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="139" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="73" borderId="139" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="143" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="143" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="75" borderId="143" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="147" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="147" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="77" borderId="147" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="151" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="151" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="79" borderId="151" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="155" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="155" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="81" borderId="155" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="159" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="159" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="83" borderId="159" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="163" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="163" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="85" borderId="163" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="167" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="167" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="87" borderId="167" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="171" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="175" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="175" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="89" borderId="175" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="179" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="179" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="91" borderId="179" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="183" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="183" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="93" borderId="183" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="187" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="187" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="166" fillId="95" borderId="187" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="191" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="191" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="97" borderId="191" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="170" fillId="0" borderId="195" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="195" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="99" borderId="195" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="199" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="199" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="175" fillId="101" borderId="199" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="203" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="203" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="103" borderId="203" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="207" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="207" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="181" fillId="105" borderId="207" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="211" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -2294,10 +3609,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3142,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9486D730-61B3-4FC6-88FC-6911F5E0A3BE}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3203,20 +4514,23 @@
         <v>83</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="101" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="103" t="s">
+      <c r="H2" s="55" t="str">
+        <f>LOWER(FALSE)</f>
+        <v>false</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="171" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="173" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3228,7 +4542,7 @@
         <v>84</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>92</v>
@@ -3236,14 +4550,17 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="34"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="104" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="106" t="s">
+      <c r="H3" s="55" t="str">
+        <f t="shared" ref="H3:H6" si="0">LOWER(FALSE)</f>
+        <v>false</v>
+      </c>
+      <c r="I3" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="174" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="176" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3255,7 +4572,7 @@
         <v>85</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>92</v>
@@ -3265,14 +4582,17 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="36"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="107" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="109" t="s">
+      <c r="H4" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I4" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="177" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="179" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3284,26 +4604,29 @@
         <v>86</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>92</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="65" t="s">
+      <c r="F5" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="110" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" s="112" t="s">
+      <c r="H5" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I5" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="180" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="182" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3315,7 +4638,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>92</v>
@@ -3323,20 +4646,23 @@
       <c r="E6" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="113" t="s">
-        <v>104</v>
-      </c>
-      <c r="K6" s="115" t="s">
+      <c r="H6" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I6" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="183" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="185" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3348,23 +4674,23 @@
         <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="42"/>
-      <c r="H7" s="60" t="str">
+      <c r="H7" s="56" t="str">
         <f>LOWER(TRUE)</f>
         <v>true</v>
       </c>
-      <c r="I7" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" s="118" t="s">
+      <c r="I7" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="186" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="188" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3376,7 +4702,7 @@
         <v>89</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>92</v>
@@ -3384,17 +4710,17 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="44"/>
-      <c r="H8" s="60" t="str">
+      <c r="H8" s="56" t="str">
         <f>LOWER(TRUE)</f>
         <v>true</v>
       </c>
-      <c r="I8" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="119" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8" s="121" t="s">
+      <c r="I8" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="189" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="191" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3406,7 +4732,7 @@
         <v>90</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>92</v>
@@ -3416,17 +4742,17 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="60" t="str">
+      <c r="H9" s="56" t="str">
         <f>LOWER(TRUE)</f>
         <v>true</v>
       </c>
-      <c r="I9" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="122" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" s="124" t="s">
+      <c r="I9" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="192" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="194" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3438,7 +4764,7 @@
         <v>91</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>92</v>
@@ -3446,29 +4772,29 @@
       <c r="E10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="60" t="str">
+      <c r="H10" s="56" t="str">
         <f>LOWER(TRUE)</f>
         <v>true</v>
       </c>
-      <c r="I10" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="125" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" s="127" t="s">
+      <c r="I10" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="195" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" s="197" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H11" s="128" t="s">
-        <v>107</v>
+      <c r="K11" s="198" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="154.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
AutomationTest-FinalProject: Backup Test Cases
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="DeleteCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="AddProject" sheetId="4" r:id="rId1"/>
+    <sheet name="EditCustomer" sheetId="2" r:id="rId2"/>
+    <sheet name="DeleteCustomer" sheetId="1" r:id="rId3"/>
+    <sheet name="EmployeeReports" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="152">
   <si>
     <t>TCs</t>
   </si>
@@ -139,14 +142,365 @@
     <t>PASSED</t>
   </si>
   <si>
+    <t>TC_OHRM_EC_01</t>
+  </si>
+  <si>
+    <t>Test that Administrator can edit customer successfully and system displays "Sucessfully Updated" with all valid required fields edited</t>
+  </si>
+  <si>
+    <t>Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Successfully Updated</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_02</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 1 character and Description has 10 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_03</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 50 characters and Description has 10 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_04</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 5 characters and Description has 0 character in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_05</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can edit customer successfully and system displays "Sucessfully Updated" with Name has 5 characters and Description has 255 characters in length</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_06</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_07</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_08</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_09</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_10</t>
+  </si>
+  <si>
+    <t>Verify that the system reloads the page and displays the Customers page when the Administrator edits invalid data into input fields then closes 'Edit Customer' form by clicking 'Cancel' button</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/time/viewCustomers</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EC_11</t>
+  </si>
+  <si>
+    <t>Verify that the system reloads the page and displays the Customers page when the Administrator edits valid data into input fields then closes 'Edit Customer' form by clicking 'Cancel' button</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Welcome To</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Company</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Saigon Tourist Saigon Tourist Saigo</t>
+  </si>
+  <si>
+    <t>Saigo</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tou</t>
+  </si>
+  <si>
+    <t>ACME Ltd</t>
+  </si>
+  <si>
+    <t>Saigon Tourist Saigon Tourist Saigon Tourist Saigon</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Required' text under customer name textbox when Administrator tries to save form with blank input to 'Name' textbox after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Already exists' text under customer name textbox when Administrator tries to save form with duplicated Name in the system after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Should not exceed 50 characters' text under customer description textbox when Administrator tries to enter on Name more than 50 characters in length after editing</t>
+  </si>
+  <si>
+    <t>Verify that system displays 'Should not exceed 255 characters' text under customer description textarea when Administrator tries to enter on Description more than 255 characters in length after editing</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Already exists</t>
+  </si>
+  <si>
+    <t>Should not exceed 50 characters</t>
+  </si>
+  <si>
+    <t>Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist Welcome To Saigon Tourist</t>
+  </si>
+  <si>
+    <t>Should not exceed 255 characters</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_01</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_02</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_03</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_04</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_05</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_06</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_07</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_08</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_09</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_10</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_11</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_12</t>
+  </si>
+  <si>
+    <t>TC_OHRM_AP_13</t>
+  </si>
+  <si>
+    <t>Test that Administrator can create a new project successfully and system displays "Sucessfully added" with all valid required fields inputted and unique Name for each Customer Name in system</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 1 character and Description has 10 characters in length and Project Admin do not blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 50 characters and Description has 10 characters in length and Project Admin do not blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters and Description has 0 character in length and Project Admin do not blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters and Description has 255 characters in length and Project Admin do not blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters, Description has 10 characters in length and Project Admin do not blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 character, Description has 10 characters in length and Project Admin is blank</t>
+  </si>
+  <si>
+    <t>Verify that Administrator cannot choose any other value than the suggested list of customers from the following system of the 'Customer Name' dropbox when entering characters</t>
+  </si>
+  <si>
+    <t>Verify that Administrator cannot choose any other value than the suggested list of customers from the following system of the 'Project Admin' dropbox when entering characters</t>
+  </si>
+  <si>
+    <t>Verify that error message displays when Administrator tries to save form with blank input to 'Name' textbox</t>
+  </si>
+  <si>
+    <t>Verify that error message displays when Administrator tries to save form with blank input to 'Customer Name' dropbox</t>
+  </si>
+  <si>
+    <t>Verify that error message displays when Administrator tries to save form with spaces only to 'Name' textbox</t>
+  </si>
+  <si>
+    <t>Verify that error message displays when Administrator tries to save form with spaces only to 'Customer Name' dropbox</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Project Description</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Project Admin</t>
+  </si>
+  <si>
+    <t>Successfully Saved</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>The project</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>The notice</t>
+  </si>
+  <si>
+    <t>Button valves for store pressure fire extinguisher</t>
+  </si>
+  <si>
+    <t>ABCDE</t>
+  </si>
+  <si>
+    <t>ABCDF</t>
+  </si>
+  <si>
+    <t>Button valves for store pressure fire extinguisher Button valves for store pressure fire extinguisher Button valves for store pressure fire extinguisher Button valves for store pressure fire extinguisher Button valves for store pressure fire extinguisher!</t>
+  </si>
+  <si>
+    <t>ABCDG</t>
+  </si>
+  <si>
+    <t>ABCDH</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>ABE</t>
+  </si>
+  <si>
+    <t>Lisa  Andrews</t>
+  </si>
+  <si>
+    <t>Chose value in the suggested list</t>
+  </si>
+  <si>
     <t>7/7</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Approved Timesheets</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_01</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee.</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>orangehrm-paper-container</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_02</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee and the project name.</t>
+  </si>
+  <si>
+    <t>ACME</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_03</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and a specific activity in the project.</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_04</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and the project date range in the project.</t>
+  </si>
+  <si>
+    <t>2023-08-13</t>
+  </si>
+  <si>
+    <t>2023-08-20</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_05</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, a specific activity, and project date range in the project.</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_06</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, and turn on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_07</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_08</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, project's activity, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>TC_OHRM_EP_09</t>
+  </si>
+  <si>
+    <t>Verify that system displays the Employee Report after the user selected an employee, the project name, the project's activity, project date range, and turns on 'Only Include Approved Timesheet'.</t>
+  </si>
+  <si>
+    <t>9/9</t>
+  </si>
+  <si>
+    <t>11/11</t>
+  </si>
+  <si>
+    <t>13/13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="69" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,12 +599,233 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +873,151 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -455,11 +1173,416 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,7 +1608,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,6 +1620,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -540,6 +1669,198 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="27" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="30" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="31" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="32" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="35" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="36" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="37" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -548,6 +1869,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FF9999FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -856,22 +2183,772 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="78" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="82" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10" s="84" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="88" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="90" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="92" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="93" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="42.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="22.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="26.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -897,7 +2974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -914,14 +2991,14 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -938,10 +3015,10 @@
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="55" t="s">
         <v>33</v>
       </c>
     </row>
@@ -964,10 +3041,10 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="57" t="s">
         <v>33</v>
       </c>
     </row>
@@ -990,10 +3067,10 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="59" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1012,10 +3089,10 @@
       <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="61" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1036,10 +3113,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="63" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1060,10 +3137,10 @@
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="65" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1077,8 +3154,8 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="27" t="s">
-        <v>34</v>
+      <c r="H9" s="66" t="s">
+        <v>119</v>
       </c>
       <c r="I9"/>
     </row>
@@ -1086,4 +3163,359 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="8" width="18.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43" t="str">
+        <f>LOWER(FALSE)</f>
+        <v>false</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43" t="str">
+        <f t="shared" ref="H3:H6" si="0">LOWER(FALSE)</f>
+        <v>false</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>false</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="47"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="43" t="str">
+        <f>LOWER(TRUE)</f>
+        <v>true</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="J11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AutomationTest-FinalProject: Update Test Case With Reporter Log
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\automation-test-group1\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddProject" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="152">
   <si>
     <t>TCs</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters and Description has 255 characters in length and Project Admin do not blank</t>
   </si>
   <si>
-    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters, Description has 10 characters in length and Project Admin do not blank</t>
-  </si>
-  <si>
     <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 character, Description has 10 characters in length and Project Admin is blank</t>
   </si>
   <si>
@@ -494,13 +491,17 @@
   </si>
   <si>
     <t>13/13</t>
+  </si>
+  <si>
+    <t>Verify that Administrator can create a new project successfully and system displays "Sucessfully added" with Name has 5 characters and Description has 10 characters in length and Project Admin do not blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="69" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="227" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,8 +825,696 @@
       <sz val="13"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="140">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1016,8 +1705,518 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="262">
     <border>
       <left/>
       <right/>
@@ -1578,11 +2777,1019 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1862,6 +4069,480 @@
     </xf>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="41" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="41" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="39" borderId="41" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="45" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="45" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="41" borderId="45" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="49" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="49" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="43" borderId="49" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="53" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="53" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="45" borderId="53" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="57" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="57" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="47" borderId="57" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="61" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="61" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="49" borderId="61" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="65" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="65" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="51" borderId="65" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="69" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="73" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="73" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="53" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="77" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="77" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="55" borderId="77" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="81" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="81" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="57" borderId="81" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="85" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="85" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="59" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="89" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="89" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="61" borderId="89" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="93" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="93" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="63" borderId="93" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="97" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="97" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="65" borderId="97" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="101" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="101" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="67" borderId="101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="105" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="105" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="69" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="109" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="109" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="71" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="113" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="113" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="73" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="117" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="117" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="75" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="121" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="121" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="77" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="125" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="125" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="79" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="129" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="129" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="81" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="133" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="133" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="83" borderId="133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="137" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="137" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="85" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="141" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="141" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="87" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="145" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="149" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="153" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="153" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="89" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="0" borderId="157" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="157" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="91" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="161" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="161" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="93" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="165" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="165" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="158" fillId="95" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="169" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="0" borderId="169" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="97" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="173" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="173" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="164" fillId="99" borderId="173" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="177" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="177" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="101" borderId="177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="181" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="181" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="170" fillId="103" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="185" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="185" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="105" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="189" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="189" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="176" fillId="107" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="193" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="193" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="109" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="197" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="181" fillId="0" borderId="197" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="111" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="183" fillId="0" borderId="201" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="201" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="185" fillId="113" borderId="201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="205" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="205" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="188" fillId="115" borderId="205" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="209" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="209" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="191" fillId="117" borderId="209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="213" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="213" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="194" fillId="119" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="217" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="196" fillId="0" borderId="217" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="197" fillId="121" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="198" fillId="0" borderId="221" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="199" fillId="0" borderId="221" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="200" fillId="123" borderId="221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="201" fillId="0" borderId="225" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="202" fillId="0" borderId="225" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="203" fillId="125" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="204" fillId="0" borderId="229" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="205" fillId="0" borderId="229" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="206" fillId="127" borderId="229" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="207" fillId="0" borderId="233" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="208" fillId="0" borderId="233" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="209" fillId="129" borderId="233" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="210" fillId="0" borderId="237" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="211" fillId="0" borderId="237" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="212" fillId="131" borderId="237" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="213" fillId="0" borderId="241" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="214" fillId="0" borderId="241" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="215" fillId="133" borderId="241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="216" fillId="0" borderId="245" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="217" fillId="0" borderId="245" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="218" fillId="135" borderId="245" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="219" fillId="0" borderId="249" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="220" fillId="0" borderId="249" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="221" fillId="137" borderId="249" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="222" fillId="0" borderId="253" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="223" fillId="0" borderId="253" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="224" fillId="139" borderId="253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="225" fillId="0" borderId="257" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="226" fillId="0" borderId="261" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2188,19 +4869,19 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -2211,16 +4892,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="F1" s="41" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>102</v>
       </c>
       <c r="G1" s="39" t="s">
         <v>3</v>
@@ -2240,24 +4921,24 @@
         <v>86</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="211" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="213" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2269,24 +4950,24 @@
         <v>87</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="214" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="216" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2298,24 +4979,24 @@
         <v>88</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="217" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="219" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2327,22 +5008,22 @@
         <v>89</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="220" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="222" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2354,24 +5035,24 @@
         <v>90</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="223" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="225" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2380,27 +5061,27 @@
         <v>78</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="226" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="228" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2409,34 +5090,34 @@
         <v>79</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="229" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="231" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2445,35 +5126,35 @@
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="232" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="234" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>81</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="83" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="84" t="s">
+      <c r="H10" s="235" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="237" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2482,25 +5163,25 @@
         <v>82</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="85" t="s">
+      <c r="H11" s="238" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="86" t="s">
+      <c r="I11" s="240" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2509,25 +5190,25 @@
         <v>83</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="87" t="s">
+      <c r="H12" s="241" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="88" t="s">
+      <c r="I12" s="243" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2536,27 +5217,27 @@
         <v>84</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="89" t="s">
+      <c r="H13" s="244" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="90" t="s">
+      <c r="I13" s="246" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2565,27 +5246,27 @@
         <v>85</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="42" t="s">
         <v>116</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>117</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="91" t="s">
+      <c r="H14" s="247" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="92" t="s">
+      <c r="I14" s="249" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2594,7 +5275,7 @@
         <v>32</v>
       </c>
       <c r="I15" s="93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2616,12 +5297,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -2669,10 +5350,10 @@
       <c r="F2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="183" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2693,10 +5374,10 @@
       <c r="F3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="186" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2717,10 +5398,10 @@
       <c r="F4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="187" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="189" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2739,10 +5420,10 @@
       <c r="F5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="148" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2763,10 +5444,10 @@
       <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="190" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="192" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2785,10 +5466,10 @@
       <c r="F7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="193" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="195" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2809,10 +5490,10 @@
       <c r="F8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="198" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2833,10 +5514,10 @@
       <c r="F9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="199" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="201" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2857,10 +5538,10 @@
       <c r="F10" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="202" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="204" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2881,10 +5562,10 @@
       <c r="F11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="205" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="207" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2905,10 +5586,10 @@
       <c r="F12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="208" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="210" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2916,8 +5597,8 @@
       <c r="G13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="51" t="s">
-        <v>150</v>
+      <c r="H13" s="251" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2932,20 +5613,20 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="26.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="42.21875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -2991,10 +5672,10 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="172" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="174" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3015,10 +5696,10 @@
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="177" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3041,10 +5722,10 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="124" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3067,10 +5748,10 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="127" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3089,10 +5770,10 @@
       <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="61" t="s">
+      <c r="H6" s="180" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3113,10 +5794,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="133" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3137,10 +5818,10 @@
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="136" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3154,8 +5835,8 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="66" t="s">
-        <v>119</v>
+      <c r="H9" s="250" t="s">
+        <v>118</v>
       </c>
       <c r="I9"/>
     </row>
@@ -3179,11 +5860,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="8" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="3" max="8" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -3194,22 +5875,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>123</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>124</v>
       </c>
       <c r="I1" s="50" t="s">
         <v>3</v>
@@ -3223,13 +5904,13 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3240,10 +5921,10 @@
         <v>false</v>
       </c>
       <c r="I2" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" s="44" t="s">
         <v>33</v>
@@ -3251,16 +5932,16 @@
     </row>
     <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="C3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="47" t="s">
         <v>130</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>131</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
@@ -3270,10 +5951,10 @@
         <v>false</v>
       </c>
       <c r="I3" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K3" s="44" t="s">
         <v>33</v>
@@ -3281,19 +5962,19 @@
     </row>
     <row r="4" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="C4" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="47" t="s">
         <v>133</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>134</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="43"/>
@@ -3302,10 +5983,10 @@
         <v>false</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K4" s="44" t="s">
         <v>33</v>
@@ -3313,33 +5994,33 @@
     </row>
     <row r="5" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="46" t="s">
-        <v>136</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>137</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="H5" s="43" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K5" s="44" t="s">
         <v>33</v>
@@ -3347,35 +6028,35 @@
     </row>
     <row r="6" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>140</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="48" t="s">
         <v>137</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="H6" s="43" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J6" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="44" t="s">
         <v>33</v>
@@ -3383,13 +6064,13 @@
     </row>
     <row r="7" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>142</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" s="47"/>
       <c r="E7" s="47"/>
@@ -3400,10 +6081,10 @@
         <v>true</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K7" s="44" t="s">
         <v>33</v>
@@ -3411,16 +6092,16 @@
     </row>
     <row r="8" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="46" t="s">
-        <v>144</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="47"/>
@@ -3430,10 +6111,10 @@
         <v>true</v>
       </c>
       <c r="I8" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K8" s="44" t="s">
         <v>33</v>
@@ -3441,19 +6122,19 @@
     </row>
     <row r="9" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>146</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="47"/>
       <c r="G9" s="43"/>
@@ -3462,10 +6143,10 @@
         <v>true</v>
       </c>
       <c r="I9" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J9" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K9" s="44" t="s">
         <v>33</v>
@@ -3473,35 +6154,35 @@
     </row>
     <row r="10" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="46" t="s">
-        <v>148</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="48" t="s">
         <v>137</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="H10" s="43" t="str">
         <f>LOWER(TRUE)</f>
         <v>true</v>
       </c>
       <c r="I10" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K10" s="44" t="s">
         <v>33</v>
@@ -3512,7 +6193,7 @@
         <v>32</v>
       </c>
       <c r="K11" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>